<commit_message>
add withdrawal report to get correct buy-dates of forex for potential transactions in the future
</commit_message>
<xml_diff>
--- a/example/tax_report_2022_daily_rates.xlsx
+++ b/example/tax_report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
   <si>
     <t>Symbol</t>
   </si>
@@ -964,7 +964,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1051,7 +1051,7 @@
         <v>41</v>
       </c>
       <c r="B4">
-        <v>3431.97</v>
+        <v>2582.03</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -1066,7 +1066,7 @@
         <v>1.03</v>
       </c>
       <c r="G4">
-        <v>76.28</v>
+        <v>57.39</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1074,22 +1074,22 @@
         <v>41</v>
       </c>
       <c r="B5">
-        <v>1825.99</v>
+        <v>849.9400000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>1.01</v>
       </c>
       <c r="F5">
-        <v>1.03</v>
+        <v>0.96</v>
       </c>
       <c r="G5">
-        <v>33.88</v>
+        <v>-43.77</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1097,166 +1097,51 @@
         <v>41</v>
       </c>
       <c r="B6">
-        <v>3088.48</v>
+        <v>150.06</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="F6">
-        <v>1.03</v>
+        <v>0.96</v>
       </c>
       <c r="G6">
-        <v>15.66</v>
+        <v>-8.279999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7">
-        <v>170</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>1.03</v>
-      </c>
-      <c r="F7">
-        <v>0.96</v>
-      </c>
-      <c r="G7">
-        <v>-11.67</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8">
-        <v>329.99</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8">
-        <v>1.01</v>
-      </c>
-      <c r="F8">
-        <v>0.96</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>-17.4</v>
+        <v>22.05</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9">
-        <v>349.99</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>1.03</v>
-      </c>
-      <c r="F9">
-        <v>0.96</v>
+        <v>14</v>
       </c>
       <c r="G9">
-        <v>-24.06</v>
+        <v>74.09999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10">
-        <v>239.99</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10">
-        <v>1.03</v>
-      </c>
-      <c r="F10">
-        <v>0.96</v>
+        <v>15</v>
       </c>
       <c r="G10">
-        <v>-16.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11">
-        <v>499.99</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11">
-        <v>0.97</v>
-      </c>
-      <c r="F11">
-        <v>0.96</v>
-      </c>
-      <c r="G11">
-        <v>-6.26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>66.64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>142.53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>-75.89</v>
+        <v>-52.05</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1627,7 @@
         <v>80</v>
       </c>
       <c r="C7">
-        <v>66.64</v>
+        <v>22.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
address further feedback, include fees specifically as part of capital gains
</commit_message>
<xml_diff>
--- a/example/tax_report_2022_daily_rates.xlsx
+++ b/example/tax_report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
   <si>
     <t>Symbol</t>
   </si>
@@ -45,6 +45,12 @@
     <t>Sell Price [EUR]</t>
   </si>
   <si>
+    <t>Gain before Costs [EUR]</t>
+  </si>
+  <si>
+    <t>Transaction Costs [EUR]</t>
+  </si>
+  <si>
     <t>Gain [EUR]</t>
   </si>
   <si>
@@ -144,9 +150,15 @@
     <t>100.00 USD</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
+    <t>2019-09-05</t>
+  </si>
+  <si>
     <t>2022-04-01</t>
   </si>
   <si>
@@ -159,7 +171,22 @@
     <t>2022-12-01</t>
   </si>
   <si>
-    <t>Comment</t>
+    <t>Held for 1133 days, no taxable gains as outside of speculative period of 1 years.</t>
+  </si>
+  <si>
+    <t>Held for 194 days, taxable gains as shorter within speculative period of 1 years.</t>
+  </si>
+  <si>
+    <t>Held for 103 days, taxable gains as shorter within speculative period of 1 years.</t>
+  </si>
+  <si>
+    <t>Held for 37 days, taxable gains as shorter within speculative period of 1 years.</t>
+  </si>
+  <si>
+    <t>Held for 87 days, taxable gains as shorter within speculative period of 1 years.</t>
+  </si>
+  <si>
+    <t>Held for 70 days, taxable gains as shorter within speculative period of 1 years.</t>
   </si>
   <si>
     <t>Date</t>
@@ -186,34 +213,7 @@
     <t>Fees</t>
   </si>
   <si>
-    <t>Fees for Sell Order (22.00 x NVDA)</t>
-  </si>
-  <si>
-    <t>Fees for Sell Order (11.00 x NVDA)</t>
-  </si>
-  <si>
-    <t>Fees for Sell Order (19.00 x NVDA)</t>
-  </si>
-  <si>
     <t>Fees for converting USD to EUR</t>
-  </si>
-  <si>
-    <t>Fees for Sell Order (3.00 x APPL)</t>
-  </si>
-  <si>
-    <t>Fees for Sell Order (2.00 x APPL)</t>
-  </si>
-  <si>
-    <t>Fees for Sell Order (5.00 x GOOG)</t>
-  </si>
-  <si>
-    <t>0.03 USD</t>
-  </si>
-  <si>
-    <t>0.01 USD</t>
-  </si>
-  <si>
-    <t>0.02 USD</t>
   </si>
   <si>
     <t>15.00 USD</t>
@@ -619,7 +619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,10 +630,12 @@
     <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,25 +663,31 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>99.86</v>
@@ -690,25 +698,31 @@
       <c r="I2">
         <v>114.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>114.79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <v>162.16</v>
@@ -719,25 +733,31 @@
       <c r="I3">
         <v>-97.98</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>0.03</v>
+      </c>
+      <c r="K3">
+        <v>-98.01000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>112.46</v>
@@ -748,25 +768,31 @@
       <c r="I4">
         <v>554.9299999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>0.01</v>
+      </c>
+      <c r="K4">
+        <v>554.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>161.52</v>
@@ -777,25 +803,31 @@
       <c r="I5">
         <v>6.43</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>161.52</v>
@@ -806,25 +838,31 @@
       <c r="I6">
         <v>271.83</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>0.02</v>
+      </c>
+      <c r="K6">
+        <v>271.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7">
         <v>125.87</v>
@@ -835,25 +873,31 @@
       <c r="I7">
         <v>-44.55</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>0.01</v>
+      </c>
+      <c r="K7">
+        <v>-44.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8">
         <v>125.87</v>
@@ -864,25 +908,31 @@
       <c r="I8">
         <v>-5.67</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>0.01</v>
+      </c>
+      <c r="K8">
+        <v>-5.68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9">
         <v>91.54000000000001</v>
@@ -893,25 +943,31 @@
       <c r="I9">
         <v>-98.81</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>0.01</v>
+      </c>
+      <c r="K9">
+        <v>-98.81999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G10">
         <v>91.54000000000001</v>
@@ -922,34 +978,40 @@
       <c r="I10">
         <v>26.87</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>0.01</v>
+      </c>
+      <c r="K10">
+        <v>26.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12">
-        <v>727.85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>727.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13">
-        <v>974.86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>974.8099999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14">
-        <v>-247.01</v>
+        <v>17</v>
+      </c>
+      <c r="K14">
+        <v>-247.07</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -975,9 +1037,10 @@
     <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -997,21 +1060,24 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>85</v>
+        <v>1247.97</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>0.9</v>
@@ -1020,90 +1086,102 @@
         <v>1.03</v>
       </c>
       <c r="G2">
-        <v>10.67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="F3">
         <v>1.03</v>
       </c>
       <c r="G3">
-        <v>6.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>10.67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>2582.03</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E4">
-        <v>1.01</v>
+        <v>0.96</v>
       </c>
       <c r="F4">
         <v>1.03</v>
       </c>
       <c r="G4">
-        <v>57.39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>6.04</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>849.9400000000001</v>
+        <v>2582.03</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E5">
         <v>1.01</v>
       </c>
       <c r="F5">
-        <v>0.96</v>
+        <v>1.03</v>
       </c>
       <c r="G5">
-        <v>-43.77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>57.39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6">
-        <v>150.06</v>
+        <v>849.9400000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>1.01</v>
@@ -1112,35 +1190,64 @@
         <v>0.96</v>
       </c>
       <c r="G6">
+        <v>-43.77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>150.06</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <v>1.01</v>
+      </c>
+      <c r="F7">
+        <v>0.96</v>
+      </c>
+      <c r="G7">
         <v>-8.279999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
         <v>22.05</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9">
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
         <v>74.09999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10">
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11">
         <v>-52.05</v>
       </c>
     </row>
@@ -1174,30 +1281,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
       <c r="E2">
         <v>90.48</v>
@@ -1205,16 +1312,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>95.92</v>
@@ -1222,12 +1329,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>186.4</v>
@@ -1245,14 +1352,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1263,182 +1370,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E2">
-        <v>0.03</v>
+        <v>15.45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>14.35</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4">
-        <v>0.02</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E5">
-        <v>15.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10">
-        <v>14.35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12">
-        <v>29.9</v>
+        <v>29.8</v>
       </c>
     </row>
   </sheetData>
@@ -1471,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1491,7 +1479,7 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>65</v>
@@ -1508,7 +1496,7 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
@@ -1519,12 +1507,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>27.96</v>
@@ -1572,7 +1560,7 @@
         <v>75</v>
       </c>
       <c r="C2">
-        <v>914.25</v>
+        <v>914.14</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1583,7 +1571,7 @@
         <v>76</v>
       </c>
       <c r="C3">
-        <v>974.86</v>
+        <v>974.8099999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1594,7 +1582,7 @@
         <v>77</v>
       </c>
       <c r="C4">
-        <v>247.01</v>
+        <v>247.07</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1616,7 +1604,7 @@
         <v>79</v>
       </c>
       <c r="C6">
-        <v>29.9</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
introduce separate fee currency column, modify accordingly, make forex gains from dividends tax-free
</commit_message>
<xml_diff>
--- a/example/tax_report_2022_daily_rates.xlsx
+++ b/example/tax_report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t>Symbol</t>
   </si>
@@ -174,10 +174,7 @@
     <t>Held for 1133 days, no taxable gains as outside of speculative period of 1 years.</t>
   </si>
   <si>
-    <t>Held for 194 days, taxable gains as shorter within speculative period of 1 years.</t>
-  </si>
-  <si>
-    <t>Held for 103 days, taxable gains as shorter within speculative period of 1 years.</t>
+    <t>FOREX not acquired (e.g. received dividend payments), thus gains not taxed.</t>
   </si>
   <si>
     <t>Held for 37 days, taxable gains as shorter within speculative period of 1 years.</t>
@@ -1071,7 +1068,7 @@
         <v>44</v>
       </c>
       <c r="B2">
-        <v>1247.97</v>
+        <v>1247.91</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1112,7 +1109,7 @@
         <v>1.03</v>
       </c>
       <c r="G3">
-        <v>10.67</v>
+        <v>0</v>
       </c>
       <c r="H3" t="s">
         <v>51</v>
@@ -1138,10 +1135,10 @@
         <v>1.03</v>
       </c>
       <c r="G4">
-        <v>6.04</v>
+        <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1149,7 +1146,7 @@
         <v>44</v>
       </c>
       <c r="B5">
-        <v>2582.03</v>
+        <v>2567.09</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1164,10 +1161,10 @@
         <v>1.03</v>
       </c>
       <c r="G5">
-        <v>57.39</v>
+        <v>57.06</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1175,7 +1172,7 @@
         <v>44</v>
       </c>
       <c r="B6">
-        <v>849.9400000000001</v>
+        <v>849.87</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -1190,10 +1187,10 @@
         <v>0.96</v>
       </c>
       <c r="G6">
-        <v>-43.77</v>
+        <v>-43.76</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1201,7 +1198,7 @@
         <v>44</v>
       </c>
       <c r="B7">
-        <v>150.06</v>
+        <v>135.13</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -1216,10 +1213,10 @@
         <v>0.96</v>
       </c>
       <c r="G7">
-        <v>-8.279999999999999</v>
+        <v>-7.45</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1232,7 +1229,7 @@
         <v>15</v>
       </c>
       <c r="G9">
-        <v>22.05</v>
+        <v>5.85</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1240,7 +1237,7 @@
         <v>16</v>
       </c>
       <c r="G10">
-        <v>74.09999999999999</v>
+        <v>57.06</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1248,7 +1245,7 @@
         <v>17</v>
       </c>
       <c r="G11">
-        <v>-52.05</v>
+        <v>-51.21</v>
       </c>
     </row>
   </sheetData>
@@ -1284,21 +1281,21 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -1312,10 +1309,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1334,7 +1331,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>186.4</v>
@@ -1373,27 +1370,27 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>15.45</v>
@@ -1401,16 +1398,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>14.35</v>
@@ -1423,7 +1420,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>29.8</v>
@@ -1462,27 +1459,27 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>13.57</v>
@@ -1490,16 +1487,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3">
         <v>14.39</v>
@@ -1512,7 +1509,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>27.96</v>
@@ -1543,21 +1540,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2">
         <v>914.14</v>
@@ -1565,10 +1562,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>974.8099999999999</v>
@@ -1576,10 +1573,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4">
         <v>247.07</v>
@@ -1587,10 +1584,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>27.96</v>
@@ -1598,10 +1595,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>29.8</v>
@@ -1609,13 +1606,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7">
-        <v>22.05</v>
+        <v>5.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate dividends and tax events during schwab export and event generation, fix a few awv-related things in the process
</commit_message>
<xml_diff>
--- a/example/tax_report_2022_daily_rates.xlsx
+++ b/example/tax_report_2022_daily_rates.xlsx
@@ -219,10 +219,10 @@
     <t>Tax Withholding</t>
   </si>
   <si>
-    <t>Withheld Tax on Dividends (NVDA)</t>
-  </si>
-  <si>
-    <t>Withheld Tax on Dividends (APPL)</t>
+    <t>Tax Withholding (NVDA)</t>
+  </si>
+  <si>
+    <t>Tax Withholding (APPL)</t>
   </si>
   <si>
     <t>ELSTER - Anlage</t>
@@ -1068,7 +1068,7 @@
         <v>44</v>
       </c>
       <c r="B2">
-        <v>1247.91</v>
+        <v>1217.91</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1094,7 +1094,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1120,7 +1120,7 @@
         <v>44</v>
       </c>
       <c r="B4">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -1445,7 +1445,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
update test and example files (APPL should always have been AAPL)
</commit_message>
<xml_diff>
--- a/example/tax_report_2022_daily_rates.xlsx
+++ b/example/tax_report_2022_daily_rates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="80">
   <si>
     <t>Symbol</t>
   </si>
@@ -51,13 +51,19 @@
     <t>Transaction Costs [EUR]</t>
   </si>
   <si>
+    <t>Buy Value [EUR]</t>
+  </si>
+  <si>
+    <t>Sell Value [EUR]</t>
+  </si>
+  <si>
     <t>Gain [EUR]</t>
   </si>
   <si>
     <t>NVDA</t>
   </si>
   <si>
-    <t>APPL</t>
+    <t>AAPL</t>
   </si>
   <si>
     <t>GOOG</t>
@@ -81,12 +87,6 @@
     <t>2020-02-28</t>
   </si>
   <si>
-    <t>2021-09-21</t>
-  </si>
-  <si>
-    <t>2022-09-21</t>
-  </si>
-  <si>
     <t>2019-10-11</t>
   </si>
   <si>
@@ -111,19 +111,13 @@
     <t>2022-11-14</t>
   </si>
   <si>
-    <t>114.00 USD</t>
-  </si>
-  <si>
-    <t>178.00 USD</t>
-  </si>
-  <si>
-    <t>132.00 USD</t>
-  </si>
-  <si>
-    <t>160.00 USD</t>
-  </si>
-  <si>
-    <t>139.00 USD</t>
+    <t>28.50 USD</t>
+  </si>
+  <si>
+    <t>44.50 USD</t>
+  </si>
+  <si>
+    <t>34.75 USD</t>
   </si>
   <si>
     <t>89.00 USD</t>
@@ -204,7 +198,7 @@
     <t>Dividend Payment (NVDA)</t>
   </si>
   <si>
-    <t>Dividend Payment (APPL)</t>
+    <t>Dividend Payment (AAPL)</t>
   </si>
   <si>
     <t>Fees</t>
@@ -222,7 +216,7 @@
     <t>Tax Withholding (NVDA)</t>
   </si>
   <si>
-    <t>Tax Withholding (APPL)</t>
+    <t>Tax Withholding (AAPL)</t>
   </si>
   <si>
     <t>ELSTER - Anlage</t>
@@ -255,10 +249,16 @@
     <t>Zeile 41: Anrechenbare noch nicht angerechnete ausländische Steuern</t>
   </si>
   <si>
-    <t>Zeile 48: (Werbungskosten Sonstiges): Überweisungsgebühren auf deutsches Konto für Gehaltsbestandteil RSU/ESPP</t>
-  </si>
-  <si>
-    <t>Zeilen 42 - 48: Gewinn / Verlust aus Verkauf von Fremdwährungen</t>
+    <t>Zeile 65: (Werbungskosten Sonstiges): Überweisungsgebühren auf deutsches Konto für Gehaltsbestandteil RSU/ESPP</t>
+  </si>
+  <si>
+    <t>Zeilen 48 - 54: Gewinn / Verlust aus Verkauf von Fremdwährungen</t>
+  </si>
+  <si>
+    <t>Zeilen 48 - 54: Veräußerungswert Fremdwährungen</t>
+  </si>
+  <si>
+    <t>Zeilen 48 - 54: Anschaffungskosten Fremdwährungen</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -625,14 +625,16 @@
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,16 +668,22 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -684,33 +692,39 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2">
-        <v>99.86</v>
+        <v>24.96</v>
       </c>
       <c r="H2">
         <v>157.26</v>
       </c>
       <c r="I2">
-        <v>114.8</v>
+        <v>1058.34</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K2">
-        <v>114.79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>199.72</v>
+      </c>
+      <c r="L2">
+        <v>1258.06</v>
+      </c>
+      <c r="M2">
+        <v>1058.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -719,202 +733,238 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3">
-        <v>162.16</v>
+        <v>40.54</v>
       </c>
       <c r="H3">
         <v>157.26</v>
       </c>
       <c r="I3">
-        <v>-97.98</v>
+        <v>1634.06</v>
       </c>
       <c r="J3">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="K3">
-        <v>-98.01000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>567.55</v>
+      </c>
+      <c r="L3">
+        <v>2201.61</v>
+      </c>
+      <c r="M3">
+        <v>1634.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4">
-        <v>112.46</v>
+        <v>40.54</v>
       </c>
       <c r="H4">
         <v>167.95</v>
       </c>
       <c r="I4">
-        <v>554.9299999999999</v>
+        <v>1401.5</v>
       </c>
       <c r="J4">
         <v>0.01</v>
       </c>
       <c r="K4">
-        <v>554.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>445.93</v>
+      </c>
+      <c r="L4">
+        <v>1847.43</v>
+      </c>
+      <c r="M4">
+        <v>1401.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>40.54</v>
+      </c>
+      <c r="H5">
+        <v>175.83</v>
+      </c>
+      <c r="I5">
+        <v>2570.43</v>
+      </c>
+      <c r="J5">
+        <v>0.02</v>
+      </c>
+      <c r="K5">
+        <v>770.25</v>
+      </c>
+      <c r="L5">
+        <v>3340.68</v>
+      </c>
+      <c r="M5">
+        <v>2570.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="G5">
-        <v>161.52</v>
-      </c>
-      <c r="H5">
-        <v>167.95</v>
-      </c>
-      <c r="I5">
-        <v>6.43</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>6.43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
       <c r="G6">
-        <v>161.52</v>
+        <v>31.47</v>
       </c>
       <c r="H6">
-        <v>175.83</v>
+        <v>111.02</v>
       </c>
       <c r="I6">
-        <v>271.83</v>
+        <v>238.66</v>
       </c>
       <c r="J6">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="K6">
-        <v>271.81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>94.40000000000001</v>
+      </c>
+      <c r="L6">
+        <v>333.06</v>
+      </c>
+      <c r="M6">
+        <v>238.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7">
-        <v>125.87</v>
+        <v>31.47</v>
       </c>
       <c r="H7">
-        <v>111.02</v>
+        <v>123.04</v>
       </c>
       <c r="I7">
-        <v>-44.55</v>
+        <v>183.14</v>
       </c>
       <c r="J7">
         <v>0.01</v>
       </c>
       <c r="K7">
-        <v>-44.56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>62.94</v>
+      </c>
+      <c r="L7">
+        <v>246.08</v>
+      </c>
+      <c r="M7">
+        <v>183.13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8">
-        <v>125.87</v>
+        <v>91.54000000000001</v>
       </c>
       <c r="H8">
-        <v>123.04</v>
+        <v>71.77</v>
       </c>
       <c r="I8">
-        <v>-5.67</v>
+        <v>-98.81</v>
       </c>
       <c r="J8">
         <v>0.01</v>
       </c>
       <c r="K8">
-        <v>-5.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>457.68</v>
+      </c>
+      <c r="L8">
+        <v>358.86</v>
+      </c>
+      <c r="M8">
+        <v>-98.81999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -923,92 +973,63 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9">
         <v>91.54000000000001</v>
       </c>
       <c r="H9">
-        <v>71.77</v>
+        <v>96.91</v>
       </c>
       <c r="I9">
-        <v>-98.81</v>
+        <v>26.87</v>
       </c>
       <c r="J9">
         <v>0.01</v>
       </c>
       <c r="K9">
+        <v>457.68</v>
+      </c>
+      <c r="L9">
+        <v>484.54</v>
+      </c>
+      <c r="M9">
+        <v>26.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11">
+        <v>7014.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12">
+        <v>7112.91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13">
         <v>-98.81999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10">
-        <v>91.54000000000001</v>
-      </c>
-      <c r="H10">
-        <v>96.91</v>
-      </c>
-      <c r="I10">
-        <v>26.87</v>
-      </c>
-      <c r="J10">
-        <v>0.01</v>
-      </c>
-      <c r="K10">
-        <v>26.86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12">
-        <v>727.74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13">
-        <v>974.8099999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14">
-        <v>-247.07</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1044,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1033,11 +1054,12 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,21 +1082,27 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1217.91</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>0.9</v>
@@ -1085,22 +1113,28 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
       <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
       </c>
       <c r="E3">
         <v>0.9</v>
@@ -1111,22 +1145,28 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>0.96</v>
@@ -1137,13 +1177,19 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>2567.09</v>
@@ -1152,7 +1198,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>1.01</v>
@@ -1161,15 +1207,21 @@
         <v>1.03</v>
       </c>
       <c r="G5">
+        <v>2587.79</v>
+      </c>
+      <c r="H5">
+        <v>2644.85</v>
+      </c>
+      <c r="I5">
         <v>57.06</v>
       </c>
-      <c r="H5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>849.87</v>
@@ -1178,7 +1230,7 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>1.01</v>
@@ -1187,15 +1239,21 @@
         <v>0.96</v>
       </c>
       <c r="G6">
+        <v>856.72</v>
+      </c>
+      <c r="H6">
+        <v>812.96</v>
+      </c>
+      <c r="I6">
         <v>-43.76</v>
       </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>135.13</v>
@@ -1204,7 +1262,7 @@
         <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>1.01</v>
@@ -1213,38 +1271,44 @@
         <v>0.96</v>
       </c>
       <c r="G7">
+        <v>136.72</v>
+      </c>
+      <c r="H7">
+        <v>129.26</v>
+      </c>
+      <c r="I7">
         <v>-7.45</v>
       </c>
-      <c r="H7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9">
+        <v>17</v>
+      </c>
+      <c r="I9">
         <v>5.85</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10">
+        <v>18</v>
+      </c>
+      <c r="I10">
         <v>57.06</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11">
+        <v>19</v>
+      </c>
+      <c r="I11">
         <v>-51.21</v>
       </c>
     </row>
@@ -1278,30 +1342,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>90.48</v>
@@ -1309,16 +1373,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>95.92</v>
@@ -1326,12 +1390,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>186.4</v>
@@ -1367,30 +1431,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
       </c>
       <c r="E2">
         <v>15.45</v>
@@ -1398,16 +1462,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
       </c>
       <c r="E3">
         <v>14.35</v>
@@ -1415,12 +1479,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>29.8</v>
@@ -1456,30 +1520,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <v>13.57</v>
@@ -1487,16 +1551,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>14.39</v>
@@ -1504,12 +1568,12 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>27.96</v>
@@ -1527,7 +1591,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1535,59 +1599,59 @@
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2">
-        <v>914.14</v>
+        <v>7200.49</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3">
-        <v>974.8099999999999</v>
+        <v>7112.91</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4">
-        <v>247.07</v>
+        <v>98.81999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>27.96</v>
@@ -1595,10 +1659,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>29.8</v>
@@ -1606,13 +1670,35 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>5.85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8">
+        <v>3587.07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>3581.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>